<commit_message>
add automatic analysis + task d + pdf
</commit_message>
<xml_diff>
--- a/Woche2/ueb2_Krien_Vosskuhl.xlsx
+++ b/Woche2/ueb2_Krien_Vosskuhl.xlsx
@@ -1,16 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\MCI1617\Woche2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10180" windowHeight="14020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10185" windowHeight="14025" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Testdaten_Mouse" sheetId="1" r:id="rId1"/>
-    <sheet name="Testdaten_Touchpad" sheetId="3" r:id="rId2"/>
+    <sheet name="Testdaten_Mouse_Automatisch" sheetId="4" r:id="rId1"/>
+    <sheet name="Testdaten_Mouse" sheetId="1" r:id="rId2"/>
+    <sheet name="Testdaten_Touchpad_Automatisch" sheetId="5" r:id="rId3"/>
+    <sheet name="Testdaten_Touchpad" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>Proband</t>
   </si>
@@ -202,6 +209,81 @@
   <si>
     <t>t-Statistik</t>
   </si>
+  <si>
+    <t>AUSGABE: ZUSAMMENFASSUNG</t>
+  </si>
+  <si>
+    <t>Regressions-Statistik</t>
+  </si>
+  <si>
+    <t>Multipler Korrelationskoeffizient</t>
+  </si>
+  <si>
+    <t>Adjustiertes Bestimmtheitsmaß</t>
+  </si>
+  <si>
+    <t>Standardfehler</t>
+  </si>
+  <si>
+    <t>Beobachtungen</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residue</t>
+  </si>
+  <si>
+    <t>Gesamt</t>
+  </si>
+  <si>
+    <t>Schnittpunkt</t>
+  </si>
+  <si>
+    <t>Freiheitsgrade (df)</t>
+  </si>
+  <si>
+    <t>Quadratsummen (SS)</t>
+  </si>
+  <si>
+    <t>Mittlere Quadratsumme (MS)</t>
+  </si>
+  <si>
+    <t>Prüfgröße (F)</t>
+  </si>
+  <si>
+    <t>F krit</t>
+  </si>
+  <si>
+    <t>Koeffizienten</t>
+  </si>
+  <si>
+    <t>P-Wert</t>
+  </si>
+  <si>
+    <t>Untere 95%</t>
+  </si>
+  <si>
+    <t>Obere 95%</t>
+  </si>
+  <si>
+    <t>Untere 95,0%</t>
+  </si>
+  <si>
+    <t>Obere 95,0%</t>
+  </si>
+  <si>
+    <t>X Variable 1</t>
+  </si>
+  <si>
+    <t>Die Statistik ist als signifikant einzustufen. In der t-Verteilungs-Tabelle findet sich der Wert 1,701 für Alpha = 0.05 und n-2 = 28. Der Wert der vorliegenden Statistik liegt mit 13.28 deutlich darüber, die Beobachtungen sind somit signifikant.</t>
+  </si>
+  <si>
+    <t>Die Statistik ist als signifikant einzustufen. In der t-Verteilungs-Tabelle findet sich der Wert 1,701 für Alpha = 0.05 und n-2 = 28. Der Wert der vorliegenden Statistik liegt mit 9.05 deutlich darüber, die Beobachtungen sind somit signifikant.</t>
+  </si>
 </sst>
 </file>
 
@@ -210,7 +292,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,6 +331,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -264,12 +354,32 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -307,16 +417,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -324,24 +431,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="32">
-    <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Dezimal" xfId="1" builtinId="3"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
@@ -361,6 +485,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -686,30 +818,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.8633773277811394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0.74542041012650107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0.73632828191673316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="10">
+        <v>91.99594661286595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10">
+        <v>693862.01625714265</v>
+      </c>
+      <c r="D12" s="10">
+        <v>693862.01625714265</v>
+      </c>
+      <c r="E12" s="10">
+        <v>81.985250639743896</v>
+      </c>
+      <c r="F12" s="10">
+        <v>8.2223103763038422E-10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="10">
+        <v>28</v>
+      </c>
+      <c r="C13" s="10">
+        <v>236971.11740952387</v>
+      </c>
+      <c r="D13" s="10">
+        <v>8463.254193197281</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="11">
+        <v>29</v>
+      </c>
+      <c r="C14" s="11">
+        <v>930833.13366666646</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="10">
+        <v>172.78266666666667</v>
+      </c>
+      <c r="C17" s="10">
+        <v>38.300966830540922</v>
+      </c>
+      <c r="D17" s="10">
+        <v>4.5111829012339966</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1.0539603422149848E-4</v>
+      </c>
+      <c r="F17" s="10">
+        <v>94.326692673323876</v>
+      </c>
+      <c r="G17" s="10">
+        <v>251.23864066000948</v>
+      </c>
+      <c r="H17" s="10">
+        <v>94.326692673323876</v>
+      </c>
+      <c r="I17" s="10">
+        <v>251.23864066000948</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="11">
+        <v>89.049714285714288</v>
+      </c>
+      <c r="C18" s="11">
+        <v>9.83478037706546</v>
+      </c>
+      <c r="D18" s="11">
+        <v>9.0545707043318124</v>
+      </c>
+      <c r="E18" s="11">
+        <v>8.2223103763038422E-10</v>
+      </c>
+      <c r="F18" s="11">
+        <v>68.904079923345677</v>
+      </c>
+      <c r="G18" s="11">
+        <v>109.1953486480829</v>
+      </c>
+      <c r="H18" s="11">
+        <v>68.904079923345677</v>
+      </c>
+      <c r="I18" s="11">
+        <v>109.1953486480829</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,7 +1108,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -780,7 +1147,7 @@
         <v>8.8067628117917511</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4">
         <v>2</v>
@@ -817,7 +1184,7 @@
         <v>1838.8740920090661</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5">
         <v>3</v>
@@ -854,7 +1221,7 @@
         <v>2221.407468988662</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6">
         <v>4</v>
@@ -891,7 +1258,7 @@
         <v>1920.0588556553189</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7">
         <v>5</v>
@@ -928,7 +1295,7 @@
         <v>19035.379261532875</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8">
         <v>6</v>
@@ -965,7 +1332,7 @@
         <v>4531.8541723355884</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1004,7 +1371,7 @@
         <v>4655.6578104308328</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10">
         <v>2</v>
@@ -1041,7 +1408,7 @@
         <v>6096.8135967709659</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11">
         <v>3</v>
@@ -1078,7 +1445,7 @@
         <v>19357.660421369616</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12">
         <v>4</v>
@@ -1115,7 +1482,7 @@
         <v>6301.4263223220032</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13">
         <v>5</v>
@@ -1152,7 +1519,7 @@
         <v>9926.3836043900301</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14">
         <v>6</v>
@@ -1189,7 +1556,7 @@
         <v>10674.82560090701</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1228,7 +1595,7 @@
         <v>6183.0513342403565</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16">
         <v>2</v>
@@ -1265,7 +1632,7 @@
         <v>8682.9028729614438</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17">
         <v>3</v>
@@ -1302,7 +1669,7 @@
         <v>2865.6546308934276</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18">
         <v>4</v>
@@ -1339,7 +1706,7 @@
         <v>6301.4263223220032</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19">
         <v>5</v>
@@ -1376,7 +1743,7 @@
         <v>90.844499628118172</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20">
         <v>6</v>
@@ -1413,7 +1780,7 @@
         <v>8515.774172335623</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -1452,7 +1819,7 @@
         <v>65008.486762811794</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22">
         <v>2</v>
@@ -1489,7 +1856,7 @@
         <v>18801.319806294799</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23">
         <v>3</v>
@@ -1526,7 +1893,7 @@
         <v>10174.391849941032</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24">
         <v>4</v>
@@ -1563,7 +1930,7 @@
         <v>5508.3822080362779</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25">
         <v>5</v>
@@ -1600,7 +1967,7 @@
         <v>1441.6268805804978</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26">
         <v>6</v>
@@ -1637,7 +2004,7 @@
         <v>32.707505668932889</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -1676,7 +2043,7 @@
         <v>9854.0601913832343</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28">
         <v>2</v>
@@ -1713,7 +2080,7 @@
         <v>6034.5079205804932</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29">
         <v>3</v>
@@ -1750,7 +2117,7 @@
         <v>165.5903261315193</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30">
         <v>4</v>
@@ -1787,7 +2154,7 @@
         <v>54.486893750567575</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31">
         <v>5</v>
@@ -1824,7 +2191,7 @@
         <v>636.61537581859704</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32">
         <v>6</v>
@@ -1861,7 +2228,7 @@
         <v>50.139886621316222</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -1887,7 +2254,7 @@
         <v>236971.11740952381</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -1911,7 +2278,7 @@
         <v>964.79693908442027</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="4"/>
@@ -1926,7 +2293,7 @@
         <v>0.86337732778113951</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1939,49 +2306,49 @@
         <v>0.74542041012650118</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="D37" s="6" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D37" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="7" t="s">
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -1993,24 +2360,25 @@
         <f>C34-B45*B34</f>
         <v>172.78266666666661</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="E45" s="14"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="7" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="8" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B48" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -2018,8 +2386,13 @@
         <f>SQRT((J33/(B48-2)))</f>
         <v>91.995946612865936</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -2027,8 +2400,11 @@
         <f>B49/SQRT(G33)</f>
         <v>9.8347803770654565</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -2036,8 +2412,11 @@
         <f>3*B50</f>
         <v>29.504341131196369</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -2045,13 +2424,17 @@
         <f>B45/B50</f>
         <v>9.054570704331816</v>
       </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D37:H41"/>
+    <mergeCell ref="C49:E52"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="38" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2060,33 +2443,260 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.92897293618625554</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0.86299071616651279</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0.85809752745817391</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="10">
+        <v>86.21813803678792</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1311026.402857143</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1311026.402857143</v>
+      </c>
+      <c r="E12" s="10">
+        <v>176.36571315874843</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1.3143478830172175E-13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="10">
+        <v>28</v>
+      </c>
+      <c r="C13" s="10">
+        <v>208139.88514285721</v>
+      </c>
+      <c r="D13" s="10">
+        <v>7433.567326530615</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="11">
+        <v>29</v>
+      </c>
+      <c r="C14" s="11">
+        <v>1519166.2880000002</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="10">
+        <v>132.2000000000001</v>
+      </c>
+      <c r="C17" s="10">
+        <v>35.895473297691829</v>
+      </c>
+      <c r="D17" s="10">
+        <v>3.6829156396302736</v>
+      </c>
+      <c r="E17" s="10">
+        <v>9.7654708404393232E-4</v>
+      </c>
+      <c r="F17" s="10">
+        <v>58.671456138887663</v>
+      </c>
+      <c r="G17" s="10">
+        <v>205.72854386111254</v>
+      </c>
+      <c r="H17" s="10">
+        <v>58.671456138887663</v>
+      </c>
+      <c r="I17" s="10">
+        <v>205.72854386111254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="11">
+        <v>122.4057142857143</v>
+      </c>
+      <c r="C18" s="11">
+        <v>9.2171066588355117</v>
+      </c>
+      <c r="D18" s="11">
+        <v>13.28027534197798</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1.3143478830172268E-13</v>
+      </c>
+      <c r="F18" s="11">
+        <v>103.52532717906713</v>
+      </c>
+      <c r="G18" s="11">
+        <v>141.28610139236147</v>
+      </c>
+      <c r="H18" s="11">
+        <v>103.52532717906713</v>
+      </c>
+      <c r="I18" s="11">
+        <v>141.28610139236147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="81" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J33"/>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2118,7 +2728,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2157,7 +2767,7 @@
         <v>2829.6320326530458</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4">
         <v>2</v>
@@ -2194,7 +2804,7 @@
         <v>4887.607844897977</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5">
         <v>3</v>
@@ -2231,7 +2841,7 @@
         <v>10509.764579591872</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6">
         <v>4</v>
@@ -2268,7 +2878,7 @@
         <v>9105.5216653061543</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7">
         <v>5</v>
@@ -2305,7 +2915,7 @@
         <v>730.54367346939603</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8">
         <v>6</v>
@@ -2342,7 +2952,7 @@
         <v>76.287746938778312</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -2381,7 +2991,7 @@
         <v>428.25346122448383</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10">
         <v>2</v>
@@ -2418,7 +3028,7 @@
         <v>2736.4855591836904</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11">
         <v>3</v>
@@ -2455,7 +3065,7 @@
         <v>23752.093722449023</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12">
         <v>4</v>
@@ -2492,7 +3102,7 @@
         <v>21176.901951020445</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13">
         <v>5</v>
@@ -2529,7 +3139,7 @@
         <v>2940.7379591836948</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14">
         <v>6</v>
@@ -2566,7 +3176,7 @@
         <v>19469.816889795951</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2605,7 +3215,7 @@
         <v>18630.690032653027</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16">
         <v>2</v>
@@ -2642,7 +3252,7 @@
         <v>11382.451273469353</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17">
         <v>3</v>
@@ -2679,7 +3289,7 @@
         <v>1081.2822938775382</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18">
         <v>4</v>
@@ -2716,7 +3326,7 @@
         <v>2359.7388081632489</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19">
         <v>5</v>
@@ -2753,7 +3363,7 @@
         <v>19285.273673469339</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20">
         <v>6</v>
@@ -2790,7 +3400,7 @@
         <v>26168.146318367333</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -2829,7 +3439,7 @@
         <v>75.789461224492399</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22">
         <v>2</v>
@@ -2866,7 +3476,7 @@
         <v>5596.7498448979841</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23">
         <v>3</v>
@@ -2903,7 +3513,7 @@
         <v>2399.3202938775344</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24">
         <v>4</v>
@@ -2940,7 +3550,7 @@
         <v>1550.5593795918289</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25">
         <v>5</v>
@@ -2977,7 +3587,7 @@
         <v>5878.5079591836393</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26">
         <v>6</v>
@@ -3014,7 +3624,7 @@
         <v>15.726889795917455</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -3053,7 +3663,7 @@
         <v>72.15288979591611</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28">
         <v>2</v>
@@ -3090,7 +3700,7 @@
         <v>212.82641632652684</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29">
         <v>3</v>
@@ -3127,7 +3737,7 @@
         <v>701.34172244897047</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30">
         <v>4</v>
@@ -3164,7 +3774,7 @@
         <v>2000.1339510204191</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31">
         <v>5</v>
@@ -3201,7 +3811,7 @@
         <v>1749.6293877551204</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32">
         <v>6</v>
@@ -3238,7 +3848,7 @@
         <v>10335.917461224453</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -3247,7 +3857,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4">
-        <f t="shared" ref="F33:I33" si="6">SUM(F3:F32)</f>
+        <f t="shared" ref="F33:H33" si="6">SUM(F3:F32)</f>
         <v>10710.5</v>
       </c>
       <c r="G33" s="4">
@@ -3264,7 +3874,7 @@
         <v>208139.88514285718</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -3288,7 +3898,7 @@
         <v>1232.5446393538857</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="4"/>
@@ -3303,7 +3913,7 @@
         <v>0.92897293618625543</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -3316,49 +3926,49 @@
         <v>0.86299071616651257</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15" customHeight="1">
-      <c r="D37" s="6" t="s">
+    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="7" t="s">
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>23</v>
       </c>
@@ -3366,7 +3976,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -3379,20 +3989,20 @@
         <v>132.20000000000016</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="7" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="8" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B48" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -3400,9 +4010,13 @@
         <f>SQRT((J33/(B48-2)))</f>
         <v>86.218138036787906</v>
       </c>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="C49" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -3410,8 +4024,11 @@
         <f>B49/SQRT(G33)</f>
         <v>9.2171066588355082</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -3419,8 +4036,11 @@
         <f>3*B50</f>
         <v>27.651319976506525</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -3428,13 +4048,17 @@
         <f>B45/B50</f>
         <v>13.280275341977983</v>
       </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D37:H41"/>
+    <mergeCell ref="C49:E52"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="37" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
weitere Beschriftungen hinzugefügt sowie Kriterien
</commit_message>
<xml_diff>
--- a/Woche2/ueb2_Krien_Vosskuhl.xlsx
+++ b/Woche2/ueb2_Krien_Vosskuhl.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\MCI1617\Woche2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10185" windowHeight="14025" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14140" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Testdaten_Mouse_Automatisch" sheetId="4" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="Testdaten_Touchpad_Automatisch" sheetId="5" r:id="rId3"/>
     <sheet name="Testdaten_Touchpad" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="86">
   <si>
     <t>Proband</t>
   </si>
@@ -279,10 +274,134 @@
     <t>X Variable 1</t>
   </si>
   <si>
-    <t>Die Statistik ist als signifikant einzustufen. In der t-Verteilungs-Tabelle findet sich der Wert 1,701 für Alpha = 0.05 und n-2 = 28. Der Wert der vorliegenden Statistik liegt mit 13.28 deutlich darüber, die Beobachtungen sind somit signifikant.</t>
-  </si>
-  <si>
-    <t>Die Statistik ist als signifikant einzustufen. In der t-Verteilungs-Tabelle findet sich der Wert 1,701 für Alpha = 0.05 und n-2 = 28. Der Wert der vorliegenden Statistik liegt mit 9.05 deutlich darüber, die Beobachtungen sind somit signifikant.</t>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>alpha (zweiseitiger Test)</t>
+  </si>
+  <si>
+    <t>alpha/2</t>
+  </si>
+  <si>
+    <t>Wert aus T-Tabelle</t>
+  </si>
+  <si>
+    <t>trkit(0,025, df=28)</t>
+  </si>
+  <si>
+    <t>S(Dach)x^2</t>
+  </si>
+  <si>
+    <t>S(Dach)x</t>
+  </si>
+  <si>
+    <t>MKrit1</t>
+  </si>
+  <si>
+    <t>MKrit2</t>
+  </si>
+  <si>
+    <t>28 Freiheitsgerade, da man N-2 berechenen muss</t>
+  </si>
+  <si>
+    <t>Man berechnet 1 durch N - 1 mal die Summe von (ID - Mittelwert ID)^2</t>
+  </si>
+  <si>
+    <t>Das ist die Wurzel von S(Dach)x^2</t>
+  </si>
+  <si>
+    <t>man nimmt den negativen kritischen Wert aus der T-Tabelle mit  P 0,975 und n 28 und multipliziert den mit S(Dach)x/Wurzel(n) und addiert 0</t>
+  </si>
+  <si>
+    <t>man nimmt den positiven kritischen Wert aus der T-Tabelle mit  P 0,975 und n 28 und multipliziert den mit S(Dach)x/Wurzel(n) und addiert 0</t>
+  </si>
+  <si>
+    <t>Die Statistik ist als signifikant einzustufen. In der t-Verteilungs-Tabelle findet sich der Wert 2,048 für Alpha = 0.05/2 und n-2 = 28. Der Wert der vorliegenden Statistik liegt mit 9.05 deutlich darüber, die Beobachtungen sind somit signifikant.</t>
+  </si>
+  <si>
+    <t>Die Statistik ist als signifikant einzustufen. In der t-Verteilungs-Tabelle findet sich der Wert 2,048 für Alpha = 0.05/2 und n-2 = 28. Der Wert der vorliegenden Statistik liegt mit 13.28 deutlich darüber, die Beobachtungen sind somit signifikant.</t>
+  </si>
+  <si>
+    <t>Ist die Wurzel von QS(e)/N-2</t>
+  </si>
+  <si>
+    <t>MSE / die Wurzel von (ID - Mittelwert ID)^2</t>
+  </si>
+  <si>
+    <t>Wurzel</t>
+  </si>
+  <si>
+    <t>3*SE(b1)</t>
+  </si>
+  <si>
+    <t>b1/SE(b1)</t>
+  </si>
+  <si>
+    <t>b1 ist (ID -Mittelwert ID)*(AVG-Mittelwert AVG) / (ID - Mittelwert ID)^2</t>
+  </si>
+  <si>
+    <t>b0 ist der Mittelwert Testadaten_Touchpad_AVG - Mittelwert Testdaten_Touchpad_ID mal b1</t>
+  </si>
+  <si>
+    <t>AVG(Dach) berechnet sich aus b0 + b1 multipliziert mit AVG</t>
+  </si>
+  <si>
+    <t>QS(e) ist das Quadrat aus dem Testwert AVG - AVG(Dach)</t>
+  </si>
+  <si>
+    <t>Der Mittelwert berchent sich aus der Summe der Testdatenwerte durch die Anzahl der Testdaten (30).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Korrelationskoeffizient berechnet sich aus der Summe von (ID -Mittelwert ID)*(AVG-Mittelwert AVG) geteilt durch  Wurzeln((ID - Mittelwert ID)^2) * Wurzel((AVG - Mittelwert AVG)^2  </t>
+  </si>
+  <si>
+    <t>Das Bestimmtheitsmaß ist das Quadrat von dem Korrelationskoeffizienten</t>
+  </si>
+  <si>
+    <t>b0 ist der Mittelwert Testadaten_Mouse_AVG - Mittelwert Testdaten_Mouse_ID mal b1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WICHTIG:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ergebnisse wurden auf 2 Kommastellen gerunden. Gerechnet wurde jedoch mit ungerundeten Werten.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -292,7 +411,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -339,6 +458,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -367,7 +506,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -375,15 +514,15 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
+  <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -416,8 +555,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -431,9 +592,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -443,29 +601,62 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="32">
-    <cellStyle name="Besuchter Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+  <cellStyles count="54">
+    <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Dezimal" xfId="1" builtinId="3"/>
     <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
@@ -481,6 +672,17 @@
     <cellStyle name="Link" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="52" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -820,263 +1022,268 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="2" spans="1:9" ht="16.5" thickBot="1"/>
+    <row r="3" spans="1:9">
+      <c r="A3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>0.8633773277811394</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>0.74542041012650107</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:9">
+      <c r="A6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>0.73632828191673316</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>91.99594661286595</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:9" ht="16.5" thickBot="1">
+      <c r="A8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="16.5" thickBot="1">
       <c r="A10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:9">
+      <c r="A12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>1</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>693862.01625714265</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>693862.01625714265</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>81.985250639743896</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>8.2223103763038422E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:9">
+      <c r="A13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>28</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>236971.11740952387</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>8463.254193197281</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" thickBot="1">
+      <c r="A14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>29</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>930833.13366666646</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12" t="s">
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" thickBot="1"/>
+    <row r="16" spans="1:9">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:9">
+      <c r="A17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>172.78266666666667</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>38.300966830540922</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>4.5111829012339966</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>1.0539603422149848E-4</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>94.326692673323876</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="9">
         <v>251.23864066000948</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="9">
         <v>94.326692673323876</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="9">
         <v>251.23864066000948</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:9" ht="16.5" thickBot="1">
+      <c r="A18" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>89.049714285714288</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>9.83478037706546</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <v>9.0545707043318124</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>8.2223103763038422E-10</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <v>68.904079923345677</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="10">
         <v>109.1953486480829</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <v>68.904079923345677</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="10">
         <v>109.1953486480829</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="70" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView view="pageLayout" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:E62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1108,7 +1315,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1147,7 +1354,7 @@
         <v>8.8067628117917511</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1"/>
       <c r="B4">
         <v>2</v>
@@ -1184,7 +1391,7 @@
         <v>1838.8740920090661</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
       <c r="B5">
         <v>3</v>
@@ -1221,7 +1428,7 @@
         <v>2221.407468988662</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1"/>
       <c r="B6">
         <v>4</v>
@@ -1258,7 +1465,7 @@
         <v>1920.0588556553189</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1"/>
       <c r="B7">
         <v>5</v>
@@ -1295,7 +1502,7 @@
         <v>19035.379261532875</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1"/>
       <c r="B8">
         <v>6</v>
@@ -1332,7 +1539,7 @@
         <v>4531.8541723355884</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1371,7 +1578,7 @@
         <v>4655.6578104308328</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1"/>
       <c r="B10">
         <v>2</v>
@@ -1408,7 +1615,7 @@
         <v>6096.8135967709659</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1"/>
       <c r="B11">
         <v>3</v>
@@ -1445,7 +1652,7 @@
         <v>19357.660421369616</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1"/>
       <c r="B12">
         <v>4</v>
@@ -1482,7 +1689,7 @@
         <v>6301.4263223220032</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1"/>
       <c r="B13">
         <v>5</v>
@@ -1519,7 +1726,7 @@
         <v>9926.3836043900301</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1"/>
       <c r="B14">
         <v>6</v>
@@ -1556,7 +1763,7 @@
         <v>10674.82560090701</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1595,7 +1802,7 @@
         <v>6183.0513342403565</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1"/>
       <c r="B16">
         <v>2</v>
@@ -1632,7 +1839,7 @@
         <v>8682.9028729614438</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1"/>
       <c r="B17">
         <v>3</v>
@@ -1669,7 +1876,7 @@
         <v>2865.6546308934276</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1"/>
       <c r="B18">
         <v>4</v>
@@ -1706,7 +1913,7 @@
         <v>6301.4263223220032</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1"/>
       <c r="B19">
         <v>5</v>
@@ -1743,7 +1950,7 @@
         <v>90.844499628118172</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1"/>
       <c r="B20">
         <v>6</v>
@@ -1780,7 +1987,7 @@
         <v>8515.774172335623</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -1819,7 +2026,7 @@
         <v>65008.486762811794</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1"/>
       <c r="B22">
         <v>2</v>
@@ -1856,7 +2063,7 @@
         <v>18801.319806294799</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1"/>
       <c r="B23">
         <v>3</v>
@@ -1893,7 +2100,7 @@
         <v>10174.391849941032</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1"/>
       <c r="B24">
         <v>4</v>
@@ -1930,7 +2137,7 @@
         <v>5508.3822080362779</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1"/>
       <c r="B25">
         <v>5</v>
@@ -1967,7 +2174,7 @@
         <v>1441.6268805804978</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1"/>
       <c r="B26">
         <v>6</v>
@@ -2004,7 +2211,7 @@
         <v>32.707505668932889</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -2043,7 +2250,7 @@
         <v>9854.0601913832343</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1"/>
       <c r="B28">
         <v>2</v>
@@ -2080,7 +2287,7 @@
         <v>6034.5079205804932</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1"/>
       <c r="B29">
         <v>3</v>
@@ -2117,7 +2324,7 @@
         <v>165.5903261315193</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1"/>
       <c r="B30">
         <v>4</v>
@@ -2154,7 +2361,7 @@
         <v>54.486893750567575</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1"/>
       <c r="B31">
         <v>5</v>
@@ -2191,7 +2398,7 @@
         <v>636.61537581859704</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1"/>
       <c r="B32">
         <v>6</v>
@@ -2228,7 +2435,7 @@
         <v>50.139886621316222</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -2254,7 +2461,7 @@
         <v>236971.11740952381</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -2277,14 +2484,24 @@
         <f>SQRT(H33)</f>
         <v>964.79693908442027</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
+      <c r="I34" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
       <c r="G35" s="5" t="s">
         <v>15</v>
       </c>
@@ -2292,12 +2509,18 @@
         <f>(F33/(G34*H34))</f>
         <v>0.86337732778113951</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="D36" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
       <c r="G36" s="5" t="s">
         <v>17</v>
       </c>
@@ -2305,54 +2528,90 @@
         <f>H35^2</f>
         <v>0.74542041012650118</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D37" s="9" t="s">
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="D37" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>22</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="2">
         <f>F33/G33</f>
         <v>89.049714285714302</v>
       </c>
@@ -2360,17 +2619,28 @@
         <f>C34-B45*B34</f>
         <v>172.78266666666661</v>
       </c>
-      <c r="E45" s="14"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D45" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+    </row>
+    <row r="46" spans="1:10">
       <c r="C46" s="3"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="7" t="s">
         <v>27</v>
       </c>
@@ -2378,21 +2648,26 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15" customHeight="1">
       <c r="A49" t="s">
         <v>29</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="2">
         <f>SQRT((J33/(B48-2)))</f>
         <v>91.995946612865936</v>
       </c>
-      <c r="C49" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C49" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -2400,11 +2675,16 @@
         <f>B49/SQRT(G33)</f>
         <v>9.8347803770654565</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C50" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -2412,11 +2692,16 @@
         <f>3*B50</f>
         <v>29.504341131196369</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C51" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -2424,20 +2709,158 @@
         <f>B45/B50</f>
         <v>9.054570704331816</v>
       </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
+      <c r="C52" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54">
+        <v>0.05</v>
+      </c>
+      <c r="C54" t="s">
+        <v>57</v>
+      </c>
+      <c r="D54">
+        <f>B54/2</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55">
+        <v>2.048</v>
+      </c>
+      <c r="C55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="3">
+        <f>(1/(B48-1))*G33</f>
+        <v>3.0172413793103448</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="2">
+        <f>SQRT(B56)</f>
+        <v>1.737020834449128</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="2">
+        <f>-B55*(B57/(SQRT(B48))+0)</f>
+        <v>-0.64949281715830387</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="2">
+        <f>B55*(B57/(SQRT(B48)))+0</f>
+        <v>0.64949281715830387</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="22"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="20">
+    <mergeCell ref="A61:E62"/>
+    <mergeCell ref="A35:B37"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="F49:H52"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="I34:I45"/>
+    <mergeCell ref="J34:J45"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="C56:F56"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="C58:H58"/>
+    <mergeCell ref="C59:H59"/>
+    <mergeCell ref="C57:F57"/>
     <mergeCell ref="D37:H41"/>
-    <mergeCell ref="C49:E52"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="38" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="38" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -2447,256 +2870,261 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="2" spans="1:9" ht="16.5" thickBot="1"/>
+    <row r="3" spans="1:9">
+      <c r="A3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>0.92897293618625554</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>0.86299071616651279</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:9">
+      <c r="A6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>0.85809752745817391</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>86.21813803678792</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:9" ht="16.5" thickBot="1">
+      <c r="A8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="16.5" thickBot="1">
       <c r="A10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:9">
+      <c r="A12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>1</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>1311026.402857143</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>1311026.402857143</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>176.36571315874843</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>1.3143478830172175E-13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:9">
+      <c r="A13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>28</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>208139.88514285721</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>7433.567326530615</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" thickBot="1">
+      <c r="A14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>29</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>1519166.2880000002</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12" t="s">
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" thickBot="1"/>
+    <row r="16" spans="1:9">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:9">
+      <c r="A17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>132.2000000000001</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>35.895473297691829</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>3.6829156396302736</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>9.7654708404393232E-4</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>58.671456138887663</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="9">
         <v>205.72854386111254</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="9">
         <v>58.671456138887663</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="9">
         <v>205.72854386111254</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:9" ht="16.5" thickBot="1">
+      <c r="A18" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>122.4057142857143</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>9.2171066588355117</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <v>13.28027534197798</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>1.3143478830172268E-13</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <v>103.52532717906713</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="10">
         <v>141.28610139236147</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <v>103.52532717906713</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="10">
         <v>141.28610139236147</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="81" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="81" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A26" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2728,7 +3156,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2767,7 +3195,7 @@
         <v>2829.6320326530458</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1"/>
       <c r="B4">
         <v>2</v>
@@ -2804,7 +3232,7 @@
         <v>4887.607844897977</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
       <c r="B5">
         <v>3</v>
@@ -2841,7 +3269,7 @@
         <v>10509.764579591872</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1"/>
       <c r="B6">
         <v>4</v>
@@ -2878,7 +3306,7 @@
         <v>9105.5216653061543</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1"/>
       <c r="B7">
         <v>5</v>
@@ -2915,7 +3343,7 @@
         <v>730.54367346939603</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1"/>
       <c r="B8">
         <v>6</v>
@@ -2952,7 +3380,7 @@
         <v>76.287746938778312</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -2991,7 +3419,7 @@
         <v>428.25346122448383</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1"/>
       <c r="B10">
         <v>2</v>
@@ -3028,7 +3456,7 @@
         <v>2736.4855591836904</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1"/>
       <c r="B11">
         <v>3</v>
@@ -3065,7 +3493,7 @@
         <v>23752.093722449023</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1"/>
       <c r="B12">
         <v>4</v>
@@ -3102,7 +3530,7 @@
         <v>21176.901951020445</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1"/>
       <c r="B13">
         <v>5</v>
@@ -3139,7 +3567,7 @@
         <v>2940.7379591836948</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1"/>
       <c r="B14">
         <v>6</v>
@@ -3176,7 +3604,7 @@
         <v>19469.816889795951</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -3215,7 +3643,7 @@
         <v>18630.690032653027</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1"/>
       <c r="B16">
         <v>2</v>
@@ -3252,7 +3680,7 @@
         <v>11382.451273469353</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1"/>
       <c r="B17">
         <v>3</v>
@@ -3289,7 +3717,7 @@
         <v>1081.2822938775382</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1"/>
       <c r="B18">
         <v>4</v>
@@ -3326,7 +3754,7 @@
         <v>2359.7388081632489</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1"/>
       <c r="B19">
         <v>5</v>
@@ -3363,7 +3791,7 @@
         <v>19285.273673469339</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1"/>
       <c r="B20">
         <v>6</v>
@@ -3400,7 +3828,7 @@
         <v>26168.146318367333</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -3439,7 +3867,7 @@
         <v>75.789461224492399</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1"/>
       <c r="B22">
         <v>2</v>
@@ -3476,7 +3904,7 @@
         <v>5596.7498448979841</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1"/>
       <c r="B23">
         <v>3</v>
@@ -3513,7 +3941,7 @@
         <v>2399.3202938775344</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1"/>
       <c r="B24">
         <v>4</v>
@@ -3550,7 +3978,7 @@
         <v>1550.5593795918289</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1"/>
       <c r="B25">
         <v>5</v>
@@ -3587,7 +4015,7 @@
         <v>5878.5079591836393</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1"/>
       <c r="B26">
         <v>6</v>
@@ -3624,7 +4052,7 @@
         <v>15.726889795917455</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -3663,7 +4091,7 @@
         <v>72.15288979591611</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1"/>
       <c r="B28">
         <v>2</v>
@@ -3700,7 +4128,7 @@
         <v>212.82641632652684</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1"/>
       <c r="B29">
         <v>3</v>
@@ -3737,7 +4165,7 @@
         <v>701.34172244897047</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1"/>
       <c r="B30">
         <v>4</v>
@@ -3774,7 +4202,7 @@
         <v>2000.1339510204191</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1"/>
       <c r="B31">
         <v>5</v>
@@ -3811,7 +4239,7 @@
         <v>1749.6293877551204</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1"/>
       <c r="B32">
         <v>6</v>
@@ -3848,7 +4276,7 @@
         <v>10335.917461224453</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -3874,7 +4302,7 @@
         <v>208139.88514285718</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -3888,7 +4316,9 @@
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
+      <c r="F34" s="17" t="s">
+        <v>74</v>
+      </c>
       <c r="G34" s="4">
         <f>SQRT(G33)</f>
         <v>9.354143466934854</v>
@@ -3897,14 +4327,24 @@
         <f>SQRT(H33)</f>
         <v>1232.5446393538857</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
+      <c r="I34" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
       <c r="G35" s="5" t="s">
         <v>15</v>
       </c>
@@ -3912,12 +4352,18 @@
         <f>(F33/(G34*H34))</f>
         <v>0.92897293618625543</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="D36" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
       <c r="G36" s="5" t="s">
         <v>17</v>
       </c>
@@ -3925,58 +4371,86 @@
         <f>H35^2</f>
         <v>0.86299071616651257</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="9" t="s">
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+    </row>
+    <row r="37" spans="1:10" ht="15" customHeight="1">
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="D37" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+    </row>
+    <row r="44" spans="1:10">
       <c r="B44" t="s">
         <v>23</v>
       </c>
       <c r="C44" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D44" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -3988,80 +4462,233 @@
         <f>C34-B45*B34</f>
         <v>132.20000000000016</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="D45" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+    <row r="49" spans="1:8">
+      <c r="A49" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B49" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:8" ht="15" customHeight="1">
+      <c r="A50" t="s">
         <v>29</v>
       </c>
-      <c r="B49">
-        <f>SQRT((J33/(B48-2)))</f>
+      <c r="B50" s="2">
+        <f>SQRT((J33/(B49-2)))</f>
         <v>86.218138036787906</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C50" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="3">
+        <f>B50/SQRT(G33)</f>
+        <v>9.2171066588355082</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="3">
+        <f>3*B51</f>
+        <v>27.651319976506525</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="3">
+        <f>B45/B51</f>
+        <v>13.280275341977983</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>30</v>
-      </c>
-      <c r="B50" s="3">
-        <f>B49/SQRT(G33)</f>
-        <v>9.2171066588355082</v>
-      </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>31</v>
-      </c>
-      <c r="B51" s="3">
-        <f>3*B50</f>
-        <v>27.651319976506525</v>
-      </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>32</v>
-      </c>
-      <c r="B52" s="3">
-        <f>B45/B50</f>
-        <v>13.280275341977983</v>
-      </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
+      <c r="B55">
+        <v>0.05</v>
+      </c>
+      <c r="C55" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55">
+        <f>B55/2</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56">
+        <v>2.048</v>
+      </c>
+      <c r="C56" t="s">
+        <v>60</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E56" s="15"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="3">
+        <f>(1/(B49-1))*G33</f>
+        <v>3.0172413793103448</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="2">
+        <f>SQRT(B57)</f>
+        <v>1.737020834449128</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" s="2">
+        <f>-B56*(B58/(SQRT(B49))+0)</f>
+        <v>-0.64949281715830387</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" s="2">
+        <f>B56*(B58/(SQRT(B49)))+0</f>
+        <v>0.64949281715830387</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="17">
+    <mergeCell ref="A35:B37"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="A62:E63"/>
+    <mergeCell ref="I34:I45"/>
+    <mergeCell ref="J34:J45"/>
+    <mergeCell ref="D36:F36"/>
     <mergeCell ref="D37:H41"/>
-    <mergeCell ref="C49:E52"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="F50:H53"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="D45:G45"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="37" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="37" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>